<commit_message>
Deploying to gh-pages from  @ 2b3d326d47503cbb358c4c8bac9a480fe3b15809 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/9.5.1.xlsx
+++ b/en/downloads/data-excel/9.5.1.xlsx
@@ -14,16 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>9.5.1 ИДП га болгон тажрыйбалык-конструктордук жумуштун жана илимий изилдөөнүн чыгымдарынын үлүшү*</t>
-  </si>
-  <si>
-    <t>9.5.1  Доля расходов на научно-исследовательские и опытно-конструкторские работы в ВВП*</t>
-  </si>
-  <si>
-    <t>9.5.1 Research and development expenditure as a proportion of GDP*</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>(пайыз менен)</t>
   </si>
@@ -52,13 +43,25 @@
     <t>Research and development expenditure as a proportion of GDP</t>
   </si>
   <si>
-    <t>*КР ФМ маалыматтары боюнча</t>
-  </si>
-  <si>
-    <t>*по данным МФ КР</t>
-  </si>
-  <si>
-    <t>* according to the MF KR</t>
+    <t>*предварительные данные</t>
+  </si>
+  <si>
+    <t>2021*</t>
+  </si>
+  <si>
+    <t>*алдын алаа маалыматтар</t>
+  </si>
+  <si>
+    <t>*preliminary data</t>
+  </si>
+  <si>
+    <t>9.5.1 ИДП га болгон тажрыйбалык-конструктордук жумуштун жана илимий изилдөөнүн чыгымдарынын үлүшү</t>
+  </si>
+  <si>
+    <t>9.5.1  Доля расходов на научно-исследовательские и опытно-конструкторские работы в ВВП</t>
+  </si>
+  <si>
+    <t>9.5.1 Research and development expenditure as a proportion of GDP</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -167,6 +170,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,11 +478,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -485,51 +489,33 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -538,154 +524,85 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2017</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2018</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2019</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2020</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
-        <v>2008</v>
-      </c>
-      <c r="E4" s="6">
-        <v>2009</v>
-      </c>
-      <c r="F4" s="6">
-        <v>2010</v>
-      </c>
-      <c r="G4" s="6">
-        <v>2011</v>
-      </c>
-      <c r="H4" s="6">
-        <v>2012</v>
-      </c>
-      <c r="I4" s="6">
-        <v>2013</v>
-      </c>
-      <c r="J4" s="6">
-        <v>2014</v>
-      </c>
-      <c r="K4" s="6">
-        <v>2015</v>
-      </c>
-      <c r="L4" s="6">
-        <v>2016</v>
-      </c>
-      <c r="M4" s="6">
-        <v>2017</v>
-      </c>
-      <c r="N4" s="6">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="D5" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="K5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="M5" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>